<commit_message>
Added modification of Excel files and some documentation for it
</commit_message>
<xml_diff>
--- a/xplmod/excel.mod/test/test2.xlsx
+++ b/xplmod/excel.mod/test/test2.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Erik\work\xatapult\xtpxlib-xoffice\xplmod\excel.mod\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F25356-C627-416C-8CD9-ACE8A737EAD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A30C73-3FDD-4CB2-8A5B-1F3EC86EED82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43790" yWindow="190" windowWidth="32710" windowHeight="18440" xr2:uid="{5D61C0D6-A385-45FF-9A1E-6C0B15B257EA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="24713" windowHeight="14586" xr2:uid="{5D61C0D6-A385-45FF-9A1E-6C0B15B257EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="EMPTYCELLNAME">Sheet1!$A$4</definedName>
+  </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>What's up?</t>
   </si>
@@ -60,6 +65,12 @@
       </rPr>
       <t>in it</t>
     </r>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt; EMPTY CELL</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -120,10 +131,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -423,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873A60E2-C6BE-4ACC-8698-6151F8048D70}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -451,6 +458,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>